<commit_message>
mmDisplayObj, use reflection for displaying and creating
</commit_message>
<xml_diff>
--- a/LungolarioMM/LungolarioMM/Test.xlsx
+++ b/LungolarioMM/LungolarioMM/Test.xlsx
@@ -13,6 +13,44 @@
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>modelname</t>
+  </si>
+  <si>
+    <t>das</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>CreateObj</t>
+  </si>
+  <si>
+    <t>ListObj</t>
+  </si>
+  <si>
+    <t>DisplayObj</t>
+  </si>
+  <si>
+    <t>DeleteObj</t>
+  </si>
+  <si>
+    <t>MODEL</t>
+  </si>
+  <si>
+    <t>CURVE</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -46,8 +84,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,75 +388,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:F16"/>
+  <dimension ref="B2:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D4" t="str">
-        <f>_xll.mmCreateObj("A","MODEL")</f>
-        <v>A:2</v>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D5" t="str">
-        <f>_xll.mmCreateObj("B","CURVE")</f>
-        <v>B:1</v>
-      </c>
-    </row>
-    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D8" t="str">
-        <f t="array" ref="D8:F11">_xll.mmListObjs()</f>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B4" t="str">
+        <f>_xll.mmCreateObj("A",C4,B6:C6)</f>
+        <v>A:4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="str">
+        <f>_xll.mmCreateObj("B",F4,E6:F7)</f>
+        <v>B:2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="array" ref="H4:J7">_xll.mmListObjs()</f>
         <v>A</v>
       </c>
-      <c r="E8" t="str">
+      <c r="I4" t="str">
         <v>MODEL</v>
       </c>
-      <c r="F8" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D9" t="str">
-        <v>A</v>
-      </c>
-      <c r="E9" t="str">
-        <v>MODEL</v>
-      </c>
-      <c r="F9" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D10" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E10" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F10" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D11" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E11" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F11" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="16" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E16" t="str">
+      <c r="J4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="array" ref="L4:N6">_xll.mmDisplayObj("A",C4)</f>
+        <v>modelname</v>
+      </c>
+      <c r="M4" t="str">
+        <v>das</v>
+      </c>
+      <c r="N4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="array" ref="P4:R6">_xll.mmDisplayObj("B",F4)</f>
+        <v>currency</v>
+      </c>
+      <c r="Q4" t="str">
+        <v>EUR</v>
+      </c>
+      <c r="R4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T4" t="str">
         <f>_xll.mmDeleteObjs()</f>
         <v>Deleted 3 object(s).</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="H5" t="str">
+        <v>B</v>
+      </c>
+      <c r="I5" t="str">
+        <v>CURVE</v>
+      </c>
+      <c r="J5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L5" t="str">
+        <v>modelname</v>
+      </c>
+      <c r="M5" t="str">
+        <v>das</v>
+      </c>
+      <c r="N5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P5" t="str">
+        <v>rate</v>
+      </c>
+      <c r="Q5" t="str">
+        <v>0.01</v>
+      </c>
+      <c r="R5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" t="str">
+        <v>modelname</v>
+      </c>
+      <c r="M6" t="str">
+        <v>das</v>
+      </c>
+      <c r="N6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R6" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J7" t="e">
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued with matrices, LINQ in GetObj
</commit_message>
<xml_diff>
--- a/LungolarioMM/LungolarioMM/Test.xlsx
+++ b/LungolarioMM/LungolarioMM/Test.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zohai\OneDrive\Documents\Visual Studio 2017\Projects\Lungolario-MM\MM\LungolarioMM\LungolarioMM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27792" windowHeight="12588"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="TestTable" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>modelname</t>
   </si>
@@ -54,12 +49,24 @@
   </si>
   <si>
     <t>CURVE</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>rates</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -152,7 +159,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -185,26 +192,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -237,23 +227,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -432,15 +405,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.3">
@@ -601,12 +574,214 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:L7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1" t="str">
+        <f>_xll.mmCreateObj(B3,C3,B5:E10)</f>
+        <v>A:1</v>
+      </c>
+      <c r="G1" t="str">
+        <f t="array" ref="G1:L7">_xll.mmDisplayObj(B1,C3)</f>
+        <v>currency</v>
+      </c>
+      <c r="H1" t="str">
+        <v>EUR</v>
+      </c>
+      <c r="I1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L1" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G2" t="str">
+        <v>rate</v>
+      </c>
+      <c r="H2" t="str">
+        <v>0</v>
+      </c>
+      <c r="I2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L2" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="str">
+        <v>rates</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Tables cannot be displayed yet</v>
+      </c>
+      <c r="I3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L3" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G4" t="str">
+        <v>name</v>
+      </c>
+      <c r="H4" t="str">
+        <v>A</v>
+      </c>
+      <c r="I4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L7" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -617,7 +792,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implementing mmDisplayObj for matrix
</commit_message>
<xml_diff>
--- a/LungolarioMM/LungolarioMM/Test.xlsx
+++ b/LungolarioMM/LungolarioMM/Test.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zohai\OneDrive\Documents\Visual Studio 2017\Projects\Lungolario-MM\MM\LungolarioMM\LungolarioMM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27792" windowHeight="12588" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="TestTable" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>modelname</t>
   </si>
@@ -66,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,7 +164,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -192,9 +197,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,6 +249,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -409,11 +448,11 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.3">
@@ -457,56 +496,56 @@
       </c>
       <c r="L4" t="str">
         <f t="array" ref="L4:N6">_xll.mmDisplayObj("A",C4)</f>
-        <v>modelName</v>
+        <v>Object not found.</v>
       </c>
       <c r="M4" t="str">
-        <v>das</v>
-      </c>
-      <c r="N4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="P4" t="str">
+        <v>Object not found.</v>
+      </c>
+      <c r="N4" t="str">
+        <v>Object not found.</v>
+      </c>
+      <c r="P4" t="e">
         <f t="array" ref="P4:R6">_xll.mmDisplayObj("B",F4)</f>
-        <v>currency</v>
-      </c>
-      <c r="Q4" t="str">
-        <v>EUR</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q4" t="e">
+        <v>#VALUE!</v>
       </c>
       <c r="R4" t="e">
-        <v>#N/A</v>
+        <v>#VALUE!</v>
       </c>
       <c r="T4" t="str">
         <f>_xll.mmDeleteObjs()</f>
-        <v>Deleted 1 object(s).</v>
+        <v>Deleted 0 object(s).</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
       <c r="H5" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="I5" t="str">
-        <v>MODEL</v>
+        <v>CURVE</v>
       </c>
       <c r="J5" t="e">
         <v>#N/A</v>
       </c>
       <c r="L5" t="str">
-        <v>extraResults</v>
+        <v>Object not found.</v>
       </c>
       <c r="M5" t="str">
-        <v>0</v>
-      </c>
-      <c r="N5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="P5" t="str">
-        <v>rate</v>
-      </c>
-      <c r="Q5" t="str">
-        <v>0.01</v>
+        <v>Object not found.</v>
+      </c>
+      <c r="N5" t="str">
+        <v>Object not found.</v>
+      </c>
+      <c r="P5" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q5" t="e">
+        <v>#VALUE!</v>
       </c>
       <c r="R5" t="e">
-        <v>#N/A</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
@@ -522,32 +561,32 @@
       <c r="F6" t="s">
         <v>4</v>
       </c>
-      <c r="H6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I6" t="e">
-        <v>#N/A</v>
+      <c r="H6" t="str">
+        <v>B</v>
+      </c>
+      <c r="I6" t="str">
+        <v>CURVE</v>
       </c>
       <c r="J6" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N6" t="e">
-        <v>#N/A</v>
+      <c r="L6" t="str">
+        <v>Object not found.</v>
+      </c>
+      <c r="M6" t="str">
+        <v>Object not found.</v>
+      </c>
+      <c r="N6" t="str">
+        <v>Object not found.</v>
       </c>
       <c r="P6" t="e">
-        <v>#N/A</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Q6" t="e">
-        <v>#N/A</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R6" t="e">
-        <v>#N/A</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
@@ -557,11 +596,11 @@
       <c r="F7" s="1">
         <v>0.01</v>
       </c>
-      <c r="H7" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I7" t="e">
-        <v>#N/A</v>
+      <c r="H7" t="str">
+        <v>B</v>
+      </c>
+      <c r="I7" t="str">
+        <v>CURVE</v>
       </c>
       <c r="J7" t="e">
         <v>#N/A</v>
@@ -576,16 +615,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B1" t="str">
         <f>_xll.mmCreateObj(B3,C3,B5:E10)</f>
-        <v>A:1</v>
+        <v>A:0</v>
       </c>
       <c r="G1" t="str">
         <f t="array" ref="G1:L7">_xll.mmDisplayObj(B1,C3)</f>
@@ -607,12 +646,12 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="G2" t="str">
         <v>rate</v>
       </c>
       <c r="H2" t="str">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I2" t="e">
         <v>#N/A</v>
@@ -627,7 +666,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -638,7 +677,7 @@
         <v>rates</v>
       </c>
       <c r="H3" t="str">
-        <v>Tables cannot be displayed yet</v>
+        <v>Tables not implemented yet.</v>
       </c>
       <c r="I3" t="e">
         <v>#N/A</v>
@@ -653,7 +692,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="G4" t="str">
         <v>name</v>
       </c>
@@ -673,7 +712,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -699,7 +738,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -722,7 +761,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>11</v>
       </c>
@@ -751,7 +790,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>1</v>
       </c>
@@ -762,7 +801,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>2</v>
       </c>
@@ -773,7 +812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>3</v>
       </c>
@@ -788,12 +827,203 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="40.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B1" t="str">
+        <f>_xll.mmCreateObj(B5,C5,B7:E12)</f>
+        <v>A:1</v>
+      </c>
+      <c r="G1" t="str">
+        <f t="array" ref="G1:L6">_xll.mmDisplayObj(B5,C5)</f>
+        <v>currency</v>
+      </c>
+      <c r="H1" t="str">
+        <v>EUR</v>
+      </c>
+      <c r="I1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K1" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L1" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="G2" t="str">
+        <v>rate</v>
+      </c>
+      <c r="H2" t="str">
+        <v>5</v>
+      </c>
+      <c r="I2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L2" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="G3" t="str">
+        <v>rates</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Tables not implemented yet.</v>
+      </c>
+      <c r="I3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L3" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="G4" t="str">
+        <v>name</v>
+      </c>
+      <c r="H4" t="str">
+        <v>A</v>
+      </c>
+      <c r="I4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="G6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Moved SaveObj(), new Unit test
</commit_message>
<xml_diff>
--- a/LungolarioMM/LungolarioMM/Test.xlsx
+++ b/LungolarioMM/LungolarioMM/Test.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zohai\OneDrive\Documents\Visual Studio 2017\Projects\Lungolario-MM\MM\LungolarioMM\LungolarioMM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Source\Repos\MM\LungolarioMM\LungolarioMM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27792" windowHeight="12588" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27792" windowHeight="12588" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,12 +123,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -137,7 +145,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -460,10 +468,10 @@
   <dimension ref="B2:T7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.44140625" customWidth="1"/>
     <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -501,7 +509,7 @@
       </c>
       <c r="H4" t="str">
         <f t="array" ref="H4:J7">_xll.mmListObjs()</f>
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I4" t="str">
         <v>CURVE</v>
@@ -511,23 +519,23 @@
       </c>
       <c r="L4" t="str">
         <f t="array" ref="L4:N6">_xll.mmDisplayObj("A",C4)</f>
-        <v>Object not found.</v>
+        <v>modelName</v>
       </c>
       <c r="M4" t="str">
-        <v>Object not found.</v>
-      </c>
-      <c r="N4" t="str">
-        <v>Object not found.</v>
-      </c>
-      <c r="P4" t="e">
+        <v>das</v>
+      </c>
+      <c r="N4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P4" t="str">
         <f t="array" ref="P4:R6">_xll.mmDisplayObj("B",F4)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q4" t="e">
-        <v>#VALUE!</v>
+        <v>currency</v>
+      </c>
+      <c r="Q4" t="str">
+        <v>EUR</v>
       </c>
       <c r="R4" t="e">
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="T4" t="str">
         <f>_xll.mmDeleteObjs()</f>
@@ -536,31 +544,31 @@
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
       <c r="H5" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="I5" t="str">
-        <v>CURVE</v>
+        <v>MODEL</v>
       </c>
       <c r="J5" t="e">
         <v>#N/A</v>
       </c>
       <c r="L5" t="str">
-        <v>Object not found.</v>
-      </c>
-      <c r="M5" t="str">
-        <v>Object not found.</v>
-      </c>
-      <c r="N5" t="str">
-        <v>Object not found.</v>
-      </c>
-      <c r="P5" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q5" t="e">
-        <v>#VALUE!</v>
+        <v>extraResults</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P5" t="str">
+        <v>rate</v>
+      </c>
+      <c r="Q5">
+        <v>0.01</v>
       </c>
       <c r="R5" t="e">
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
@@ -585,23 +593,23 @@
       <c r="J6" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L6" t="str">
-        <v>Object not found.</v>
-      </c>
-      <c r="M6" t="str">
-        <v>Object not found.</v>
-      </c>
-      <c r="N6" t="str">
-        <v>Object not found.</v>
+      <c r="L6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M6" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N6" t="e">
+        <v>#N/A</v>
       </c>
       <c r="P6" t="e">
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="Q6" t="e">
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="R6" t="e">
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
@@ -611,11 +619,11 @@
       <c r="F7" s="1">
         <v>0.01</v>
       </c>
-      <c r="H7" t="str">
-        <v>B</v>
-      </c>
-      <c r="I7" t="str">
-        <v>CURVE</v>
+      <c r="H7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I7" t="e">
+        <v>#N/A</v>
       </c>
       <c r="J7" t="e">
         <v>#N/A</v>
@@ -630,16 +638,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B1" t="str">
         <f>_xll.mmCreateObj(B3,C3,B5:E10)</f>
-        <v>A:0</v>
+        <v>A:3</v>
       </c>
       <c r="G1" t="str">
         <f t="array" ref="G1:L7">_xll.mmDisplayObj(B1,C3)</f>
@@ -648,11 +656,11 @@
       <c r="H1" t="str">
         <v>EUR</v>
       </c>
-      <c r="I1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J1" t="e">
-        <v>#N/A</v>
+      <c r="I1" t="str">
+        <v/>
+      </c>
+      <c r="J1" t="str">
+        <v/>
       </c>
       <c r="K1" t="e">
         <v>#N/A</v>
@@ -665,14 +673,14 @@
       <c r="G2" t="str">
         <v>rate</v>
       </c>
-      <c r="H2" t="str">
+      <c r="H2">
         <v>5</v>
       </c>
-      <c r="I2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J2" t="e">
-        <v>#N/A</v>
+      <c r="I2" t="str">
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <v/>
       </c>
       <c r="K2" t="e">
         <v>#N/A</v>
@@ -692,13 +700,13 @@
         <v>rates</v>
       </c>
       <c r="H3" t="str">
-        <v>Tables not implemented yet.</v>
-      </c>
-      <c r="I3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J3" t="e">
-        <v>#N/A</v>
+        <v/>
+      </c>
+      <c r="I3" t="str">
+        <v/>
+      </c>
+      <c r="J3" t="str">
+        <v/>
       </c>
       <c r="K3" t="e">
         <v>#N/A</v>
@@ -709,16 +717,16 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="G4" t="str">
-        <v>name</v>
+        <v/>
       </c>
       <c r="H4" t="str">
         <v>A</v>
       </c>
-      <c r="I4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J4" t="e">
-        <v>#N/A</v>
+      <c r="I4" t="str">
+        <v>B</v>
+      </c>
+      <c r="J4" t="str">
+        <v>C</v>
       </c>
       <c r="K4" t="e">
         <v>#N/A</v>
@@ -734,17 +742,17 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J5" t="e">
-        <v>#N/A</v>
+      <c r="G5" t="str">
+        <v/>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
       </c>
       <c r="K5" t="e">
         <v>#N/A</v>
@@ -757,17 +765,17 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J6" t="e">
-        <v>#N/A</v>
+      <c r="G6" t="str">
+        <v/>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
       </c>
       <c r="K6" t="e">
         <v>#N/A</v>
@@ -844,300 +852,302 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="40.88671875" customWidth="1"/>
+    <col min="1" max="7" width="8.88671875" style="2"/>
+    <col min="8" max="8" width="40.88671875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B1" t="str">
+      <c r="B1" s="2" t="str">
         <f>_xll.mmCreateObj(B5,C5,B7:E12)</f>
-        <v>A:3</v>
-      </c>
-      <c r="G1" t="str">
+        <v>A:2</v>
+      </c>
+      <c r="G1" s="2" t="str">
         <f t="array" ref="G1:L6">_xll.mmDisplayObj(B5,C5)</f>
         <v>currency</v>
       </c>
-      <c r="H1" t="str">
+      <c r="H1" s="2" t="str">
         <v>EUR</v>
       </c>
-      <c r="I1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L1" t="e">
+      <c r="I1" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J1" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K1" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L1" s="2" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="G2" t="str">
+      <c r="G2" s="2" t="str">
         <v>rate</v>
       </c>
-      <c r="H2" t="str">
+      <c r="H2" s="2" t="str">
         <v>5</v>
       </c>
-      <c r="I2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L2" t="e">
+      <c r="I2" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K2" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L2" s="2" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="G3" t="str">
+      <c r="G3" s="2" t="str">
         <v>rates</v>
       </c>
-      <c r="H3" t="str">
+      <c r="H3" s="2" t="str">
         <v>Tables not implemented yet.</v>
       </c>
-      <c r="I3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L3" t="e">
+      <c r="I3" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J3" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K3" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L3" s="2" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="G4" t="str">
+      <c r="G4" s="2" t="str">
         <v>name</v>
       </c>
-      <c r="H4" t="str">
+      <c r="H4" s="2" t="str">
         <v>A</v>
       </c>
-      <c r="I4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L4" t="e">
+      <c r="I4" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J4" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K4" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L4" s="2" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L5" t="e">
+      <c r="G5" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H5" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I5" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J5" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K5" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L5" s="2" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="G6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L6" t="e">
+      <c r="G6" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H6" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I6" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J6" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K6" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" s="2" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C10">
+      <c r="C10" s="2">
         <v>1</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>3</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C11">
+      <c r="C11" s="2">
         <v>2</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>4</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="H14" t="s">
+      <c r="H14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I15" t="s">
+      <c r="I15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I16" t="s">
+      <c r="I16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="I17" t="s">
+      <c r="I17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H19" t="s">
+      <c r="H19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="I20" t="s">
+      <c r="I20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="I21" t="s">
+      <c r="I21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="I22" t="s">
+      <c r="I22" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="23" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="J23" t="s">
+      <c r="J23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L23" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="J24">
+      <c r="J24" s="2">
         <v>1</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="2">
         <v>2</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="J25">
+      <c r="J25" s="2">
         <v>4</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="2">
         <v>5</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="2">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rewrote mmLoadObjs() and mmSaveObjs()
</commit_message>
<xml_diff>
--- a/LungolarioMM/LungolarioMM/Test.xlsx
+++ b/LungolarioMM/LungolarioMM/Test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27792" windowHeight="12588" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27792" windowHeight="12588"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,10 +130,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -465,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T7"/>
+  <dimension ref="B2:T11"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,6 +637,12 @@
         <v>#N/A</v>
       </c>
     </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="H11" t="str">
+        <f>_xll.mmSaveObjs(H4:H6,I4:I6,"test6.txt")</f>
+        <v>3 object(s) was/were saved!</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -638,208 +652,211 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B1" t="str">
+      <c r="B1" s="3" t="str">
         <f>_xll.mmCreateObj(B3,C3,B5:E10)</f>
-        <v>A:3</v>
-      </c>
-      <c r="G1" t="str">
+        <v>A:0</v>
+      </c>
+      <c r="G1" s="3" t="str">
         <f t="array" ref="G1:L7">_xll.mmDisplayObj(B1,C3)</f>
         <v>currency</v>
       </c>
-      <c r="H1" t="str">
+      <c r="H1" s="3" t="str">
         <v>EUR</v>
       </c>
-      <c r="I1" t="str">
+      <c r="I1" s="3" t="str">
         <v/>
       </c>
-      <c r="J1" t="str">
+      <c r="J1" s="3" t="str">
         <v/>
       </c>
-      <c r="K1" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L1" t="e">
+      <c r="K1" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L1" s="3" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="G2" t="str">
+      <c r="G2" s="3" t="str">
         <v>rate</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>5</v>
       </c>
-      <c r="I2" t="str">
+      <c r="I2" s="3" t="str">
         <v/>
       </c>
-      <c r="J2" t="str">
+      <c r="J2" s="3" t="str">
         <v/>
       </c>
-      <c r="K2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L2" t="e">
+      <c r="K2" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L2" s="3" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="str">
+      <c r="G3" s="3" t="str">
         <v>rates</v>
       </c>
-      <c r="H3" t="str">
+      <c r="H3" s="3" t="str">
         <v/>
       </c>
-      <c r="I3" t="str">
+      <c r="I3" s="3" t="str">
         <v/>
       </c>
-      <c r="J3" t="str">
+      <c r="J3" s="3" t="str">
         <v/>
       </c>
-      <c r="K3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L3" t="e">
+      <c r="K3" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L3" s="3" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="G4" t="str">
+      <c r="G4" s="3" t="str">
         <v/>
       </c>
-      <c r="H4" t="str">
+      <c r="H4" s="3" t="str">
         <v>A</v>
       </c>
-      <c r="I4" t="str">
+      <c r="I4" s="3" t="str">
         <v>B</v>
       </c>
-      <c r="J4" t="str">
+      <c r="J4" s="3" t="str">
         <v>C</v>
       </c>
-      <c r="K4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L4" t="e">
+      <c r="K4" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L4" s="3" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G5" t="str">
+      <c r="G5" s="3" t="str">
         <v/>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <v>1</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
         <v>3</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="3">
         <v>5</v>
       </c>
-      <c r="K5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L5" t="e">
+      <c r="K5" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L5" s="3" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="str">
+      <c r="G6" s="3" t="str">
         <v/>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>2</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="3">
         <v>4</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="3">
         <v>6</v>
       </c>
-      <c r="K6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L6" t="e">
+      <c r="K6" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" s="3" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G7" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H7" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I7" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J7" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K7" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L7" t="e">
+      <c r="G7" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H7" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I7" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J7" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K7" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L7" s="3" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C8">
+      <c r="C8" s="3">
         <v>1</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>3</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C9">
+      <c r="C9" s="3">
         <v>2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>4</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Handling of nullable in Creation, Handling of Missing in Creation, started bootstrapper
</commit_message>
<xml_diff>
--- a/LungolarioMM/LungolarioMM/Test.xlsx
+++ b/LungolarioMM/LungolarioMM/Test.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Source\Repos\MM\LungolarioMM\LungolarioMM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27792" windowHeight="12588"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="TestTable" sheetId="2" r:id="rId2"/>
     <sheet name="TestSheetFor Saving MatrixData" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>modelname</t>
   </si>
@@ -81,12 +76,21 @@
   </si>
   <si>
     <t>number 2.</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>contrate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -130,14 +134,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -153,7 +158,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -195,7 +200,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -228,26 +233,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -280,23 +268,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -475,15 +446,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.3">
@@ -656,9 +627,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.3">
@@ -869,21 +840,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="8.88671875" style="2"/>
-    <col min="8" max="8" width="40.88671875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="7" width="8.85546875" style="2"/>
+    <col min="8" max="8" width="40.85546875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="str">
         <f>_xll.mmCreateObj(B5,C5,B7:E12)</f>
-        <v>A:2</v>
+        <v>Invalid cast from 'System.Double' to 'System.Nullable`1[[System.Double, mscorlib, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089]]'.</v>
       </c>
       <c r="G1" s="2" t="str">
         <f t="array" ref="G1:L6">_xll.mmDisplayObj(B5,C5)</f>
@@ -905,7 +876,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G2" s="2" t="str">
         <v>rate</v>
       </c>
@@ -925,7 +896,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G3" s="2" t="str">
         <v>rates</v>
       </c>
@@ -945,7 +916,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G4" s="2" t="str">
         <v>name</v>
       </c>
@@ -965,7 +936,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
@@ -991,7 +962,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="G6" s="2" t="e">
         <v>#N/A</v>
       </c>
@@ -1011,7 +982,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1019,26 +990,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>14</v>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C10" s="2">
         <v>1</v>
       </c>
@@ -1049,7 +1020,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C11" s="2">
         <v>2</v>
       </c>
@@ -1060,7 +1031,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
@@ -1068,7 +1039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="H14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1079,7 +1050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="I15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1087,7 +1058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="I16" s="2" t="s">
         <v>12</v>
       </c>
@@ -1095,7 +1066,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="I17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1103,7 +1074,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="H19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1114,7 +1085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="I20" s="2" t="s">
         <v>3</v>
       </c>
@@ -1122,7 +1093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="I21" s="2" t="s">
         <v>17</v>
       </c>
@@ -1130,12 +1101,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="I22" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="J23" s="2" t="s">
         <v>11</v>
       </c>
@@ -1146,7 +1117,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="8:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="J24" s="2">
         <v>1</v>
       </c>
@@ -1157,7 +1128,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="8:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="J25" s="2">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Implemented Bootstrapper with KeyValuePair
</commit_message>
<xml_diff>
--- a/LungolarioMM/LungolarioMM/Test.xlsx
+++ b/LungolarioMM/LungolarioMM/Test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t>modelname</t>
   </si>
@@ -134,12 +134,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -841,7 +842,7 @@
   <dimension ref="B1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +855,7 @@
     <row r="1" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="str">
         <f>_xll.mmCreateObj(B5,C5,B7:E12)</f>
-        <v>Invalid cast from 'System.Double' to 'System.Nullable`1[[System.Double, mscorlib, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089]]'.</v>
+        <v>A:8</v>
       </c>
       <c r="G1" s="2" t="str">
         <f t="array" ref="G1:L6">_xll.mmDisplayObj(B5,C5)</f>
@@ -1011,35 +1012,32 @@
     </row>
     <row r="10" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
         <v>1</v>
       </c>
-      <c r="D10" s="2">
-        <v>3</v>
-      </c>
-      <c r="E10" s="2">
-        <v>5</v>
+      <c r="E10" s="5">
+        <v>0.05</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
         <v>2</v>
       </c>
-      <c r="D11" s="2">
-        <v>4</v>
-      </c>
-      <c r="E11" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="2">
-        <v>5</v>
-      </c>
-    </row>
+      <c r="E11" s="5">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="14.45" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="str">
+        <f>_xll.mmCurveDF(B1,3)</f>
+        <v>Sequence contains no elements</v>
+      </c>
       <c r="H14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1051,6 +1049,10 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B15" s="2">
+        <f>_xll.mmCurveRate(B1,D10,D11)</f>
+        <v>9.999999999999995E-3</v>
+      </c>
       <c r="I15" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Set private Properties to null when modified
</commit_message>
<xml_diff>
--- a/LungolarioMM/LungolarioMM/Test.xlsx
+++ b/LungolarioMM/LungolarioMM/Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -445,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T11"/>
+  <dimension ref="B2:T13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,6 +613,12 @@
       <c r="H11" t="str">
         <f>_xll.mmSaveObjs(H4:H6,I4:I6,"test6.txt")</f>
         <v>3 object(s) was/were saved!</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="E13" t="str">
+        <f>_xll.mmModifyObj(E4,F4,E6,F6)</f>
+        <v>B:1</v>
       </c>
     </row>
   </sheetData>
@@ -841,7 +847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
MMA finsihed, implemented enums
</commit_message>
<xml_diff>
--- a/LungolarioMM/LungolarioMM/Test.xlsx
+++ b/LungolarioMM/LungolarioMM/Test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>modelname</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>contrate</t>
+  </si>
+  <si>
+    <t>Bootstrap</t>
+  </si>
+  <si>
+    <t>NORMAL</t>
   </si>
 </sst>
 </file>
@@ -448,7 +454,7 @@
   <dimension ref="B2:T13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,8 +487,8 @@
         <v>9</v>
       </c>
       <c r="E4" t="str">
-        <f>_xll.mmCreateObj("B",F4,E6:F7)</f>
-        <v>B:0</v>
+        <f>_xll.mmCreateObj("B",F4,E6:F8)</f>
+        <v>Enums not implemented yet!</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -607,6 +613,14 @@
       </c>
       <c r="J7" t="e">
         <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.3">
@@ -618,7 +632,7 @@
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E13" t="str">
         <f>_xll.mmModifyObj(E4,F4,E6,F6)</f>
-        <v>B:1</v>
+        <v>Object not found.</v>
       </c>
     </row>
   </sheetData>

</xml_diff>